<commit_message>
Edit test case e2e_e02, add PDF website element guide from coda.io
</commit_message>
<xml_diff>
--- a/cypress/fixtures/testCase/testCase_e2eTest.xlsx
+++ b/cypress/fixtures/testCase/testCase_e2eTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\awika-portfolio\automationpractice\cypress\fixtures\testCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5560851E-2B01-4FE4-AD24-6500DEB8E12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79003578-F8E3-4904-992A-CD6C4EB9A553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="553" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="553" firstSheet="8" activeTab="13" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
   </bookViews>
   <sheets>
     <sheet name="column_ref" sheetId="2" r:id="rId1"/>
@@ -244,13 +244,13 @@
     <t>productDetailIcon[2], productDetailInput[5], productDetailIcon[3]</t>
   </si>
   <si>
-    <t>shopingCartSummaryInput[2], shopingCartSummaryIcon[3]</t>
-  </si>
-  <si>
     <t>quickview</t>
   </si>
   <si>
     <t>shopingCartSummaryIcon[2], shopingCartSummaryInput[3]</t>
+  </si>
+  <si>
+    <t>shopingCartSummaryInput[2], shopingCartSummaryIcon[1]</t>
   </si>
 </sst>
 </file>
@@ -735,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C6351B-47AC-4A85-A3FB-088019320162}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -1481,7 +1481,7 @@
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
       <c r="L3" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
@@ -1497,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97896865-25CA-4438-97F9-39EAD5C92FCA}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1653,7 +1653,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>36</v>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="K4" s="20"/>
       <c r="L4" s="21" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
@@ -2002,7 +2002,7 @@
         <v>29</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>31</v>
@@ -2582,7 +2582,7 @@
         <v>30</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J4" s="28" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Edit word 'process' to 'proceed'
</commit_message>
<xml_diff>
--- a/cypress/fixtures/testCase/testCase_e2eTest.xlsx
+++ b/cypress/fixtures/testCase/testCase_e2eTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\awika-portfolio\automationpractice\cypress\fixtures\testCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79003578-F8E3-4904-992A-CD6C4EB9A553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834410FC-64E4-4BC0-8067-84CF99E70C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="553" firstSheet="8" activeTab="13" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="553" activeTab="1" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
   </bookViews>
   <sheets>
     <sheet name="column_ref" sheetId="2" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>addToCartFrom</t>
   </si>
   <si>
-    <t>processToCheckoutFrom</t>
-  </si>
-  <si>
     <t>deletedThisOrderFrom</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>shopingCartSummaryInput[2], shopingCartSummaryIcon[1]</t>
+  </si>
+  <si>
+    <t>proceedToCheckoutFrom</t>
   </si>
 </sst>
 </file>
@@ -736,7 +736,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -760,10 +760,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -784,22 +784,22 @@
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
@@ -819,34 +819,34 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="M2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -904,7 +904,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -939,21 +939,21 @@
         <v>1</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="11">
         <v>1</v>
@@ -968,13 +968,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1032,7 +1032,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -1067,28 +1067,28 @@
         <v>1</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
       <c r="L2" s="21"/>
       <c r="M2" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -1102,27 +1102,27 @@
         <v>1</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="27">
         <v>2</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
       <c r="L3" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="4" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="27">
         <v>1</v>
@@ -1145,16 +1145,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
       <c r="K4" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="21"/>
@@ -1216,7 +1216,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -1251,28 +1251,28 @@
         <v>1</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
       <c r="L2" s="21"/>
       <c r="M2" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -1286,27 +1286,27 @@
         <v>1</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="27">
         <v>2</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
       <c r="L3" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
@@ -1314,7 +1314,7 @@
     </row>
     <row r="4" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="27">
         <v>1</v>
@@ -1329,16 +1329,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
       <c r="K4" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="21"/>
@@ -1398,7 +1398,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -1433,30 +1433,30 @@
         <v>1</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="18">
         <v>1</v>
@@ -1471,17 +1471,17 @@
         <v>3</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
       <c r="L3" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
@@ -1497,7 +1497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97896865-25CA-4438-97F9-39EAD5C92FCA}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -1543,7 +1543,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -1578,28 +1578,28 @@
         <v>1</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
       <c r="L2" s="21"/>
       <c r="M2" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -1613,27 +1613,27 @@
         <v>1</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="18">
         <v>3</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
       <c r="L3" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="4" spans="1:15" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="18">
         <v>2</v>
@@ -1650,25 +1650,25 @@
         <v>1</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="18">
         <v>1</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" s="20"/>
       <c r="L4" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
@@ -1684,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A8D453-88BA-4430-BEC2-9D2C3EA6C8DE}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1728,7 +1728,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -1763,30 +1763,30 @@
         <v>1</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="24" t="s">
         <v>30</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>31</v>
       </c>
       <c r="K2" s="24"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1798,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B69174E-A0C4-4E0C-AF6E-BA1D4DA99AB2}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1842,7 +1842,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -1871,38 +1871,38 @@
         <v>1</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="18">
         <v>3</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="20"/>
       <c r="L2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1914,7 +1914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC548CCA-358C-4232-9928-77B69EA705DF}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -1958,7 +1958,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -1987,38 +1987,38 @@
         <v>1</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="18">
         <v>3</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="20"/>
       <c r="L2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2031,7 +2031,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2075,7 +2075,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -2110,28 +2110,28 @@
         <v>1</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
       <c r="L2" s="21"/>
       <c r="M2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="21" t="s">
-        <v>49</v>
-      </c>
       <c r="O2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -2145,29 +2145,29 @@
         <v>1</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="27">
         <v>2</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" s="28"/>
       <c r="L3" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
@@ -2227,7 +2227,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -2256,36 +2256,36 @@
         <v>5</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="30">
+        <v>1</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="30">
-        <v>1</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="H2" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>30</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>31</v>
       </c>
       <c r="K2" s="28"/>
       <c r="L2" s="21"/>
       <c r="M2" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2298,7 +2298,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2341,7 +2341,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -2370,38 +2370,38 @@
         <v>5</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>41</v>
-      </c>
       <c r="H2" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K2" s="28"/>
       <c r="L2" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2414,7 +2414,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2458,7 +2458,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -2493,28 +2493,28 @@
         <v>1</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
       <c r="L2" s="21"/>
       <c r="M2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="21" t="s">
         <v>48</v>
-      </c>
-      <c r="N2" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -2528,29 +2528,29 @@
         <v>1</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="27">
         <v>2</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" s="28"/>
       <c r="L3" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
@@ -2567,29 +2567,29 @@
         <v>5</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="27">
         <v>3</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K4" s="28"/>
       <c r="L4" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
@@ -2650,7 +2650,7 @@
         <v>addToCartFrom</v>
       </c>
       <c r="J1" s="9" t="str">
-        <v>processToCheckoutFrom</v>
+        <v>proceedToCheckoutFrom</v>
       </c>
       <c r="K1" s="9" t="str">
         <v>deletedThisOrderFrom</v>
@@ -2685,21 +2685,21 @@
         <v>1</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="11">
         <v>1</v>
@@ -2714,13 +2714,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>